<commit_message>
chore: progressing cyber police
</commit_message>
<xml_diff>
--- a/projects/cyber police/api_analysis_mapping.xlsx
+++ b/projects/cyber police/api_analysis_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Still_going\Content\cyber_police\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF13B5F-B3F6-4C26-8F03-EC12221664C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92143F79-7280-49AA-BB81-CCD2789FFB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>sub analysis</t>
   </si>
@@ -96,6 +96,46 @@
   </si>
   <si>
     <t>get_users_mentions</t>
+  </si>
+  <si>
+    <t>case usage</t>
+  </si>
+  <si>
+    <t>2. keyword extraction</t>
+  </si>
+  <si>
+    <t>1. group by day overtime</t>
+  </si>
+  <si>
+    <t>x axis</t>
+  </si>
+  <si>
+    <t>y axis</t>
+  </si>
+  <si>
+    <t>✔</t>
+  </si>
+  <si>
+    <t>attr</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>retweet_count
+quote_count</t>
+  </si>
+  <si>
+    <t>like_count</t>
+  </si>
+  <si>
+    <t>reply_count</t>
+  </si>
+  <si>
+    <t>created_at</t>
   </si>
 </sst>
 </file>
@@ -139,21 +179,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,149 +478,244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.77734375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="7" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="E2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+      <c r="E3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
+      <c r="E4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+      <c r="E5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
+      <c r="E6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="E7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
+      <c r="H8" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
+      <c r="H9" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="G10" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="B11" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+    <row r="17" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H1048576" xr:uid="{3346FC01-D320-438E-9C40-F00316022311}">
+      <formula1>"✔"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -586,7 +725,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9566225-4F24-4862-A7AA-FB435239201F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>

<commit_message>
[chore]: progressing cyber police
</commit_message>
<xml_diff>
--- a/projects/cyber police/api_analysis_mapping.xlsx
+++ b/projects/cyber police/api_analysis_mapping.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\AIly\projects\cyber police\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F880ECBF-56D5-4856-858D-D16ED89D4464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76410363-888F-4334-9FB3-857B43AD8B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="56">
   <si>
     <t>sub analysis</t>
   </si>
@@ -162,6 +163,55 @@
   <si>
     <t>8️⃣Cyber Police Account Online Activities
 🐤➡📊</t>
+  </si>
+  <si>
+    <t>get_liked_tweets</t>
+  </si>
+  <si>
+    <t>expansions=['author_id']</t>
+  </si>
+  <si>
+    <t>metric author username tweet</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>7. user composition</t>
+  </si>
+  <si>
+    <t>5. keyword extraction</t>
+  </si>
+  <si>
+    <t>6. group by day overtime</t>
+  </si>
+  <si>
+    <t>8. keyword extraction</t>
+  </si>
+  <si>
+    <t>9. group by day overtime</t>
+  </si>
+  <si>
+    <t>10. user composition</t>
+  </si>
+  <si>
+    <t>expansions=['referenced_tweets.id.author_id']</t>
+  </si>
+  <si>
+    <t>11. keyword extraction</t>
+  </si>
+  <si>
+    <t>12. group by day overtime</t>
+  </si>
+  <si>
+    <t>13. user composition</t>
+  </si>
+  <si>
+    <t>14. group by day overtime</t>
+  </si>
+  <si>
+    <t>14. group by day overtime
+15. total</t>
   </si>
 </sst>
 </file>
@@ -257,6 +307,187 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>390750</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114493</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{881A405E-65EF-7D8A-1B36-DC5F7AAADBDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1609950" cy="1381318"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>48312</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>124853</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86AA259D-D9C3-68E1-5304-D777A2E1ED5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="0"/>
+          <a:ext cx="4925112" cy="7363853"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>429451</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>77297</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92B98AE6-BC5E-301D-1B76-1625B50CE745}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7315200" y="0"/>
+          <a:ext cx="5915851" cy="7859222"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>219446</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171752</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80626EAD-030D-25B8-FD1C-383DB86C5241}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13411200" y="0"/>
+          <a:ext cx="2657846" cy="2162477"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -522,21 +753,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="8.88671875" style="6" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" hidden="1"/>
   </cols>
@@ -746,135 +977,388 @@
       <c r="B11" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="C11" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="E11" s="5" t="s">
         <v>21</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="C12" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="E12" s="5" t="s">
         <v>22</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="C13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E13" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="F13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="C15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="F15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="C16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
+      <c r="F16" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="C17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="5" t="s">
+      <c r="F17" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="C18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
+      <c r="F18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="C20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="F20" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="C21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="5" t="s">
+      <c r="F21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="C22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="5" t="s">
+      <c r="F22" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="C23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="5" t="s">
+      <c r="F23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="C25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="F25" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="5" t="s">
+      <c r="C26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="5" t="s">
+      <c r="C27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B28" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="5" t="s">
+      <c r="C28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B29" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="5" t="s">
+      <c r="C29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B30" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="5" t="s">
+      <c r="C30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="5" t="s">
         <v>8</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -886,4 +1370,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB0A3A9-7E33-47ED-BF07-5D95E4C0D04A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[chore]: cyber police progressing
</commit_message>
<xml_diff>
--- a/projects/cyber police/api_analysis_mapping.xlsx
+++ b/projects/cyber police/api_analysis_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\AIly\projects\cyber police\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76410363-888F-4334-9FB3-857B43AD8B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85537DBB-1875-4B7F-AFF4-FD7B81DF3111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -235,12 +235,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -264,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -291,6 +315,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -757,7 +793,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -802,7 +838,7 @@
       <c r="A2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -974,7 +1010,7 @@
       <c r="A11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1070,7 +1106,7 @@
       <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -1166,7 +1202,7 @@
       <c r="A21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="13" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -1262,7 +1298,7 @@
       <c r="A26" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -1291,7 +1327,7 @@
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="5" t="s">
@@ -1308,7 +1344,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="13" t="s">
         <v>32</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -1325,7 +1361,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="5" t="s">

</xml_diff>